<commit_message>
Adding Use Cases Diagram to Documents
</commit_message>
<xml_diff>
--- a/Documents/Gantt-chart.xlsx
+++ b/Documents/Gantt-chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6924DC4A-8205-4B57-8A43-76B524B2CDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3589E8B6-3004-470C-A611-97D8AD212636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,12 +1103,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1145,6 +1139,12 @@
     <xf numFmtId="37" fontId="0" fillId="13" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1161,24 +1161,31 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border>
-        <left/>
         <right/>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -1205,89 +1212,10 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1418,44 +1346,14 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="8" tint="-0.499984740745262"/>
+        <b/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1497,31 +1395,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1691,22 +1564,22 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="5" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="40"/>
-      <tableStyleElement type="headerRow" dxfId="39"/>
-      <tableStyleElement type="firstRowStripe" dxfId="38"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="37"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="31"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="27"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="35"/>
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="totalRow" dxfId="33"/>
-      <tableStyleElement type="firstColumn" dxfId="32"/>
-      <tableStyleElement type="lastColumn" dxfId="31"/>
-      <tableStyleElement type="firstRowStripe" dxfId="30"/>
-      <tableStyleElement type="secondRowStripe" dxfId="29"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="totalRow" dxfId="24"/>
+      <tableStyleElement type="firstColumn" dxfId="23"/>
+      <tableStyleElement type="lastColumn" dxfId="22"/>
+      <tableStyleElement type="firstRowStripe" dxfId="21"/>
+      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1926,9 +1799,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>222250</xdr:colOff>
+          <xdr:colOff>215900</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>355600</xdr:rowOff>
+          <xdr:rowOff>361950</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2024,7 +1897,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8EE7DA96-2148-4820-AB9C-230AD0CA6702}" name="Milestones34" displayName="Milestones34" ref="B8:F34" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8EE7DA96-2148-4820-AB9C-230AD0CA6702}" name="Milestones34" displayName="Milestones34" ref="B8:F34" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="B8:F34" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2049,7 +1922,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35262E6B-D397-41BC-8148-E03FF3C288A5}" name="Milestones3" displayName="Milestones3" ref="B8:F38" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35262E6B-D397-41BC-8148-E03FF3C288A5}" name="Milestones3" displayName="Milestones3" ref="B8:F38" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B8:F38" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2074,7 +1947,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Milestones" displayName="Milestones" ref="B8:F34" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Milestones" displayName="Milestones" ref="B8:F34" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="B8:F34" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2605,7 +2478,7 @@
       </c>
       <c r="C5" s="51">
         <f ca="1">IFERROR(IF(MIN(Milestones34[Start])=0,TODAY(),MIN(Milestones34[Start])),TODAY())</f>
-        <v>45888</v>
+        <v>45912</v>
       </c>
       <c r="E5" s="67"/>
       <c r="H5" s="34"/>
@@ -2614,18 +2487,18 @@
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
       <c r="M5" s="36"/>
-      <c r="O5" s="106" t="s">
+      <c r="O5" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="107">
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="119">
         <v>13</v>
       </c>
-      <c r="V5" s="107"/>
+      <c r="V5" s="119"/>
     </row>
     <row r="6" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
@@ -2651,7 +2524,7 @@
       <c r="N6" s="27"/>
       <c r="O6" s="27" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>October</v>
       </c>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
@@ -2691,7 +2564,7 @@
       <c r="AP6" s="27"/>
       <c r="AQ6" s="27" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v>October</v>
+        <v/>
       </c>
       <c r="AR6" s="27"/>
       <c r="AS6" s="27"/>
@@ -2701,7 +2574,7 @@
       <c r="AW6" s="27"/>
       <c r="AX6" s="27" t="str">
         <f ca="1">IF(OR(TEXT(AX7,"mmmm")=AQ6,TEXT(AX7,"mmmm")=AJ6,TEXT(AX7,"mmmm")=AC6,TEXT(AX7,"mmmm")=V6),"",TEXT(AX7,"mmmm"))</f>
-        <v/>
+        <v>November</v>
       </c>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="27"/>
@@ -2725,227 +2598,227 @@
       <c r="B7" s="23"/>
       <c r="H7" s="97">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>45901</v>
+        <v>45925</v>
       </c>
       <c r="I7" s="98">
         <f ca="1">H7+1</f>
-        <v>45902</v>
+        <v>45926</v>
       </c>
       <c r="J7" s="98">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>45903</v>
+        <v>45927</v>
       </c>
       <c r="K7" s="98">
         <f ca="1">J7+1</f>
-        <v>45904</v>
+        <v>45928</v>
       </c>
       <c r="L7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45905</v>
+        <v>45929</v>
       </c>
       <c r="M7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="N7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45907</v>
+        <v>45931</v>
       </c>
       <c r="O7" s="98">
         <f ca="1">N7+1</f>
-        <v>45908</v>
+        <v>45932</v>
       </c>
       <c r="P7" s="98">
         <f ca="1">O7+1</f>
-        <v>45909</v>
+        <v>45933</v>
       </c>
       <c r="Q7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45910</v>
+        <v>45934</v>
       </c>
       <c r="R7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45911</v>
+        <v>45935</v>
       </c>
       <c r="S7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45912</v>
+        <v>45936</v>
       </c>
       <c r="T7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45913</v>
+        <v>45937</v>
       </c>
       <c r="U7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45914</v>
+        <v>45938</v>
       </c>
       <c r="V7" s="98">
         <f ca="1">U7+1</f>
-        <v>45915</v>
+        <v>45939</v>
       </c>
       <c r="W7" s="98">
         <f ca="1">V7+1</f>
-        <v>45916</v>
+        <v>45940</v>
       </c>
       <c r="X7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45917</v>
+        <v>45941</v>
       </c>
       <c r="Y7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45918</v>
+        <v>45942</v>
       </c>
       <c r="Z7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45919</v>
+        <v>45943</v>
       </c>
       <c r="AA7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45920</v>
+        <v>45944</v>
       </c>
       <c r="AB7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45921</v>
+        <v>45945</v>
       </c>
       <c r="AC7" s="98">
         <f ca="1">AB7+1</f>
-        <v>45922</v>
+        <v>45946</v>
       </c>
       <c r="AD7" s="98">
         <f ca="1">AC7+1</f>
-        <v>45923</v>
+        <v>45947</v>
       </c>
       <c r="AE7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45924</v>
+        <v>45948</v>
       </c>
       <c r="AF7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45925</v>
+        <v>45949</v>
       </c>
       <c r="AG7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45926</v>
+        <v>45950</v>
       </c>
       <c r="AH7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45927</v>
+        <v>45951</v>
       </c>
       <c r="AI7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45928</v>
+        <v>45952</v>
       </c>
       <c r="AJ7" s="98">
         <f ca="1">AI7+1</f>
-        <v>45929</v>
+        <v>45953</v>
       </c>
       <c r="AK7" s="98">
         <f ca="1">AJ7+1</f>
-        <v>45930</v>
+        <v>45954</v>
       </c>
       <c r="AL7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45931</v>
+        <v>45955</v>
       </c>
       <c r="AM7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45932</v>
+        <v>45956</v>
       </c>
       <c r="AN7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45933</v>
+        <v>45957</v>
       </c>
       <c r="AO7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45934</v>
+        <v>45958</v>
       </c>
       <c r="AP7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45935</v>
+        <v>45959</v>
       </c>
       <c r="AQ7" s="98">
         <f ca="1">AP7+1</f>
-        <v>45936</v>
+        <v>45960</v>
       </c>
       <c r="AR7" s="98">
         <f ca="1">AQ7+1</f>
-        <v>45937</v>
+        <v>45961</v>
       </c>
       <c r="AS7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45938</v>
+        <v>45962</v>
       </c>
       <c r="AT7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45939</v>
+        <v>45963</v>
       </c>
       <c r="AU7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45940</v>
+        <v>45964</v>
       </c>
       <c r="AV7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45941</v>
+        <v>45965</v>
       </c>
       <c r="AW7" s="98">
         <f t="shared" ca="1" si="0"/>
-        <v>45942</v>
+        <v>45966</v>
       </c>
       <c r="AX7" s="98">
         <f ca="1">AW7+1</f>
-        <v>45943</v>
+        <v>45967</v>
       </c>
       <c r="AY7" s="98">
         <f ca="1">AX7+1</f>
-        <v>45944</v>
+        <v>45968</v>
       </c>
       <c r="AZ7" s="98">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>45945</v>
+        <v>45969</v>
       </c>
       <c r="BA7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>45946</v>
+        <v>45970</v>
       </c>
       <c r="BB7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>45947</v>
+        <v>45971</v>
       </c>
       <c r="BC7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>45948</v>
+        <v>45972</v>
       </c>
       <c r="BD7" s="98">
         <f t="shared" ca="1" si="1"/>
-        <v>45949</v>
+        <v>45973</v>
       </c>
       <c r="BE7" s="98">
         <f ca="1">BD7+1</f>
-        <v>45950</v>
+        <v>45974</v>
       </c>
       <c r="BF7" s="98">
         <f ca="1">BE7+1</f>
-        <v>45951</v>
+        <v>45975</v>
       </c>
       <c r="BG7" s="98">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>45952</v>
+        <v>45976</v>
       </c>
       <c r="BH7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>45953</v>
+        <v>45977</v>
       </c>
       <c r="BI7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>45954</v>
+        <v>45978</v>
       </c>
       <c r="BJ7" s="98">
         <f t="shared" ca="1" si="2"/>
-        <v>45955</v>
+        <v>45979</v>
       </c>
       <c r="BK7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45956</v>
+        <v>45980</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="31" customHeight="1" x14ac:dyDescent="0.35">
@@ -2968,227 +2841,227 @@
       <c r="G8" s="103"/>
       <c r="H8" s="94" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="I8" s="95" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="J8" s="95" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="K8" s="95" t="str">
         <f t="shared" ref="K8:BK8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="L8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="M8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="N8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="O8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="P8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="Q8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="R8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="S8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="T8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="U8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="V8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="W8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="X8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="Y8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="Z8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AA8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AB8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AC8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AD8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AE8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AF8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AG8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AH8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AI8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AJ8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AK8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AL8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AM8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AN8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AO8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AP8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AQ8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AR8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AS8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AT8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AU8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AV8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AW8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AX8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AY8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AZ8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BA8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BB8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BC8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BD8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BE8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="BF8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="BG8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BH8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BI8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BJ8" s="95" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BK8" s="96" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3500,7 +3373,7 @@
       </c>
       <c r="E11" s="46">
         <f ca="1">TODAY()</f>
-        <v>45891</v>
+        <v>45915</v>
       </c>
       <c r="F11" s="16">
         <v>3</v>
@@ -3740,7 +3613,7 @@
       <c r="D12" s="93"/>
       <c r="E12" s="46">
         <f ca="1">TODAY()+5</f>
-        <v>45896</v>
+        <v>45920</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
@@ -3982,7 +3855,7 @@
       </c>
       <c r="E13" s="46">
         <f ca="1">TODAY()-3</f>
-        <v>45888</v>
+        <v>45912</v>
       </c>
       <c r="F13" s="16">
         <v>10</v>
@@ -4222,7 +4095,7 @@
       <c r="D14" s="93"/>
       <c r="E14" s="46">
         <f ca="1">TODAY()+20</f>
-        <v>45911</v>
+        <v>45935</v>
       </c>
       <c r="F14" s="16">
         <v>1</v>
@@ -4464,7 +4337,7 @@
       </c>
       <c r="E15" s="46">
         <f ca="1">TODAY()+6</f>
-        <v>45897</v>
+        <v>45921</v>
       </c>
       <c r="F15" s="16">
         <v>6</v>
@@ -4941,7 +4814,7 @@
       </c>
       <c r="E17" s="46">
         <f ca="1">TODAY()+6</f>
-        <v>45897</v>
+        <v>45921</v>
       </c>
       <c r="F17" s="16">
         <v>13</v>
@@ -5183,7 +5056,7 @@
       </c>
       <c r="E18" s="46">
         <f ca="1">TODAY()+7</f>
-        <v>45898</v>
+        <v>45922</v>
       </c>
       <c r="F18" s="16">
         <v>9</v>
@@ -5425,7 +5298,7 @@
       </c>
       <c r="E19" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F19" s="16">
         <v>11</v>
@@ -5665,7 +5538,7 @@
       <c r="D20" s="93"/>
       <c r="E20" s="46">
         <f ca="1">TODAY()+24</f>
-        <v>45915</v>
+        <v>45939</v>
       </c>
       <c r="F20" s="16">
         <v>1</v>
@@ -5905,7 +5778,7 @@
       <c r="D21" s="93"/>
       <c r="E21" s="46">
         <f ca="1">TODAY()+25</f>
-        <v>45916</v>
+        <v>45940</v>
       </c>
       <c r="F21" s="16">
         <v>24</v>
@@ -6380,7 +6253,7 @@
       <c r="D23" s="93"/>
       <c r="E23" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F23" s="16">
         <v>4</v>
@@ -6620,7 +6493,7 @@
       <c r="D24" s="93"/>
       <c r="E24" s="46">
         <f ca="1">TODAY()+19</f>
-        <v>45910</v>
+        <v>45934</v>
       </c>
       <c r="F24" s="16">
         <v>14</v>
@@ -6860,7 +6733,7 @@
       <c r="D25" s="93"/>
       <c r="E25" s="46">
         <f ca="1">TODAY()+35</f>
-        <v>45926</v>
+        <v>45950</v>
       </c>
       <c r="F25" s="16">
         <v>6</v>
@@ -7100,7 +6973,7 @@
       <c r="D26" s="93"/>
       <c r="E26" s="46">
         <f ca="1">TODAY()+48</f>
-        <v>45939</v>
+        <v>45963</v>
       </c>
       <c r="F26" s="16">
         <v>3</v>
@@ -7340,7 +7213,7 @@
       <c r="D27" s="93"/>
       <c r="E27" s="46">
         <f ca="1">TODAY()+40</f>
-        <v>45931</v>
+        <v>45955</v>
       </c>
       <c r="F27" s="16">
         <v>19</v>
@@ -7815,7 +7688,7 @@
       <c r="D29" s="93"/>
       <c r="E29" s="46">
         <f ca="1">TODAY()+37</f>
-        <v>45928</v>
+        <v>45952</v>
       </c>
       <c r="F29" s="16">
         <v>15</v>
@@ -8055,7 +7928,7 @@
       <c r="D30" s="93"/>
       <c r="E30" s="46">
         <f ca="1">TODAY()+29</f>
-        <v>45920</v>
+        <v>45944</v>
       </c>
       <c r="F30" s="16">
         <v>5</v>
@@ -8295,7 +8168,7 @@
       <c r="D31" s="93"/>
       <c r="E31" s="46">
         <f ca="1">TODAY()+80</f>
-        <v>45971</v>
+        <v>45995</v>
       </c>
       <c r="F31" s="16">
         <v>5</v>
@@ -9324,17 +9197,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:BK34">
-    <cfRule type="expression" dxfId="23" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BK34">
-    <cfRule type="expression" dxfId="22" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="5" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E9+1,H$7&lt;=$E9+$F9-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK8">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>H$7&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9457,8 +9330,8 @@
   </sheetPr>
   <dimension ref="A1:BK38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="67" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="67" zoomScaleNormal="89" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -9635,7 +9508,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="51">
-        <v>45708</v>
+        <v>45707</v>
       </c>
       <c r="E5" s="67"/>
       <c r="H5" s="37"/>
@@ -9644,18 +9517,18 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
       <c r="M5" s="39"/>
-      <c r="O5" s="106" t="s">
+      <c r="O5" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="107">
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="119">
         <v>0</v>
       </c>
-      <c r="V5" s="107"/>
+      <c r="V5" s="119"/>
     </row>
     <row r="6" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
@@ -9752,227 +9625,227 @@
       <c r="B7" s="23"/>
       <c r="H7" s="55">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>45708</v>
+        <v>45707</v>
       </c>
       <c r="I7" s="56">
         <f ca="1">H7+1</f>
-        <v>45709</v>
+        <v>45708</v>
       </c>
       <c r="J7" s="56">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>45710</v>
+        <v>45709</v>
       </c>
       <c r="K7" s="56">
         <f ca="1">J7+1</f>
-        <v>45711</v>
+        <v>45710</v>
       </c>
       <c r="L7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45712</v>
+        <v>45711</v>
       </c>
       <c r="M7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45713</v>
+        <v>45712</v>
       </c>
       <c r="N7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45714</v>
+        <v>45713</v>
       </c>
       <c r="O7" s="56">
         <f ca="1">N7+1</f>
-        <v>45715</v>
+        <v>45714</v>
       </c>
       <c r="P7" s="56">
         <f ca="1">O7+1</f>
-        <v>45716</v>
+        <v>45715</v>
       </c>
       <c r="Q7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45717</v>
+        <v>45716</v>
       </c>
       <c r="R7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45718</v>
+        <v>45717</v>
       </c>
       <c r="S7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45719</v>
+        <v>45718</v>
       </c>
       <c r="T7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45720</v>
+        <v>45719</v>
       </c>
       <c r="U7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45721</v>
+        <v>45720</v>
       </c>
       <c r="V7" s="56">
         <f ca="1">U7+1</f>
-        <v>45722</v>
+        <v>45721</v>
       </c>
       <c r="W7" s="56">
         <f ca="1">V7+1</f>
-        <v>45723</v>
+        <v>45722</v>
       </c>
       <c r="X7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45724</v>
+        <v>45723</v>
       </c>
       <c r="Y7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45725</v>
+        <v>45724</v>
       </c>
       <c r="Z7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45726</v>
+        <v>45725</v>
       </c>
       <c r="AA7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45727</v>
+        <v>45726</v>
       </c>
       <c r="AB7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45728</v>
+        <v>45727</v>
       </c>
       <c r="AC7" s="56">
         <f ca="1">AB7+1</f>
-        <v>45729</v>
+        <v>45728</v>
       </c>
       <c r="AD7" s="56">
         <f ca="1">AC7+1</f>
-        <v>45730</v>
+        <v>45729</v>
       </c>
       <c r="AE7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45731</v>
+        <v>45730</v>
       </c>
       <c r="AF7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45732</v>
+        <v>45731</v>
       </c>
       <c r="AG7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45733</v>
+        <v>45732</v>
       </c>
       <c r="AH7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45734</v>
+        <v>45733</v>
       </c>
       <c r="AI7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45735</v>
+        <v>45734</v>
       </c>
       <c r="AJ7" s="56">
         <f ca="1">AI7+1</f>
-        <v>45736</v>
+        <v>45735</v>
       </c>
       <c r="AK7" s="56">
         <f ca="1">AJ7+1</f>
-        <v>45737</v>
+        <v>45736</v>
       </c>
       <c r="AL7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45738</v>
+        <v>45737</v>
       </c>
       <c r="AM7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45739</v>
+        <v>45738</v>
       </c>
       <c r="AN7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45740</v>
+        <v>45739</v>
       </c>
       <c r="AO7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45741</v>
+        <v>45740</v>
       </c>
       <c r="AP7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45742</v>
+        <v>45741</v>
       </c>
       <c r="AQ7" s="56">
         <f ca="1">AP7+1</f>
-        <v>45743</v>
+        <v>45742</v>
       </c>
       <c r="AR7" s="56">
         <f ca="1">AQ7+1</f>
-        <v>45744</v>
+        <v>45743</v>
       </c>
       <c r="AS7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45745</v>
+        <v>45744</v>
       </c>
       <c r="AT7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45746</v>
+        <v>45745</v>
       </c>
       <c r="AU7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45747</v>
+        <v>45746</v>
       </c>
       <c r="AV7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45748</v>
+        <v>45747</v>
       </c>
       <c r="AW7" s="56">
         <f t="shared" ca="1" si="0"/>
-        <v>45749</v>
+        <v>45748</v>
       </c>
       <c r="AX7" s="56">
         <f ca="1">AW7+1</f>
-        <v>45750</v>
+        <v>45749</v>
       </c>
       <c r="AY7" s="56">
         <f ca="1">AX7+1</f>
-        <v>45751</v>
+        <v>45750</v>
       </c>
       <c r="AZ7" s="56">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>45752</v>
+        <v>45751</v>
       </c>
       <c r="BA7" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>45753</v>
+        <v>45752</v>
       </c>
       <c r="BB7" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>45754</v>
+        <v>45753</v>
       </c>
       <c r="BC7" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>45755</v>
+        <v>45754</v>
       </c>
       <c r="BD7" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>45756</v>
+        <v>45755</v>
       </c>
       <c r="BE7" s="56">
         <f ca="1">BD7+1</f>
-        <v>45757</v>
+        <v>45756</v>
       </c>
       <c r="BF7" s="56">
         <f ca="1">BE7+1</f>
-        <v>45758</v>
+        <v>45757</v>
       </c>
       <c r="BG7" s="56">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>45759</v>
+        <v>45758</v>
       </c>
       <c r="BH7" s="56">
         <f t="shared" ca="1" si="2"/>
-        <v>45760</v>
+        <v>45759</v>
       </c>
       <c r="BI7" s="56">
         <f t="shared" ca="1" si="2"/>
-        <v>45761</v>
+        <v>45760</v>
       </c>
       <c r="BJ7" s="56">
         <f t="shared" ca="1" si="2"/>
-        <v>45762</v>
+        <v>45761</v>
       </c>
       <c r="BK7" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>45763</v>
+        <v>45762</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="31" customHeight="1" x14ac:dyDescent="0.35">
@@ -9995,15 +9868,15 @@
       <c r="G8" s="72"/>
       <c r="H8" s="57" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="I8" s="54" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="J8" s="54" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="K8" s="54" t="str">
         <f t="shared" ref="K8:BK8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
@@ -10011,27 +9884,27 @@
       </c>
       <c r="L8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="M8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="N8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="O8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="P8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="Q8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="R8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10039,27 +9912,27 @@
       </c>
       <c r="S8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="T8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="U8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="V8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="W8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="X8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="Y8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10067,27 +9940,27 @@
       </c>
       <c r="Z8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AA8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AB8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AC8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AD8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AE8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AF8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10095,27 +9968,27 @@
       </c>
       <c r="AG8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AH8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AI8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AJ8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AK8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AL8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AM8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10123,27 +9996,27 @@
       </c>
       <c r="AN8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AO8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AP8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AQ8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AR8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AS8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AT8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10151,27 +10024,27 @@
       </c>
       <c r="AU8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AV8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AW8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="AX8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="AY8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AZ8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BA8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10179,27 +10052,27 @@
       </c>
       <c r="BB8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BC8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BD8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="BE8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>W</v>
       </c>
       <c r="BF8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BG8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BH8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10207,15 +10080,15 @@
       </c>
       <c r="BI8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BJ8" s="54" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BK8" s="71" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -10283,13 +10156,13 @@
     </row>
     <row r="10" spans="1:63" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
-      <c r="B10" s="115" t="s">
+      <c r="B10" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="116"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="119"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="117"/>
       <c r="G10" s="31"/>
       <c r="H10" s="30" t="str">
         <f>IFERROR(IF(LEN(Milestones3[[#This Row],[Days]])=0,"",IF(AND(H$7=$E10,$F10=1),Milestone_Marker,"")),"")</f>
@@ -10518,21 +10391,21 @@
     </row>
     <row r="11" spans="1:63" s="1" customFormat="1" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="109"/>
-      <c r="D11" s="112">
+      <c r="C11" s="107"/>
+      <c r="D11" s="110">
         <v>1</v>
       </c>
-      <c r="E11" s="113">
-        <v>45708</v>
-      </c>
-      <c r="F11" s="110">
-        <v>7</v>
+      <c r="E11" s="111">
+        <v>45707</v>
+      </c>
+      <c r="F11" s="108">
+        <v>8</v>
       </c>
       <c r="G11" s="31"/>
-      <c r="H11" s="108" t="str">
+      <c r="H11" s="106" t="str">
         <f ca="1">IFERROR(IF(LEN(Milestones3[[#This Row],[Days]])=0,"",IF(AND(H$7=$E11,$F11=1),Milestone_Marker,"")),"")</f>
         <v/>
       </c>
@@ -10759,17 +10632,17 @@
     </row>
     <row r="12" spans="1:63" s="1" customFormat="1" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="109"/>
-      <c r="D12" s="114">
+      <c r="C12" s="107"/>
+      <c r="D12" s="112">
         <v>1</v>
       </c>
-      <c r="E12" s="113">
+      <c r="E12" s="111">
         <v>45708</v>
       </c>
-      <c r="F12" s="110">
+      <c r="F12" s="108">
         <v>3</v>
       </c>
       <c r="G12" s="31"/>
@@ -11244,7 +11117,7 @@
       </c>
       <c r="E14" s="46">
         <f ca="1">TODAY()+6</f>
-        <v>45897</v>
+        <v>45921</v>
       </c>
       <c r="F14" s="16">
         <v>13</v>
@@ -11486,7 +11359,7 @@
       </c>
       <c r="E15" s="46">
         <f ca="1">TODAY()+7</f>
-        <v>45898</v>
+        <v>45922</v>
       </c>
       <c r="F15" s="16">
         <v>9</v>
@@ -11728,7 +11601,7 @@
       </c>
       <c r="E16" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F16" s="16">
         <v>11</v>
@@ -11968,7 +11841,7 @@
       <c r="D17" s="48"/>
       <c r="E17" s="46">
         <f ca="1">TODAY()+24</f>
-        <v>45915</v>
+        <v>45939</v>
       </c>
       <c r="F17" s="16">
         <v>1</v>
@@ -12208,7 +12081,7 @@
       <c r="D18" s="92"/>
       <c r="E18" s="46">
         <f ca="1">TODAY()+25</f>
-        <v>45916</v>
+        <v>45940</v>
       </c>
       <c r="F18" s="16">
         <v>24</v>
@@ -13382,7 +13255,7 @@
       <c r="D23" s="92"/>
       <c r="E23" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F23" s="16">
         <v>4</v>
@@ -13622,7 +13495,7 @@
       <c r="D24" s="48"/>
       <c r="E24" s="46">
         <f ca="1">TODAY()+19</f>
-        <v>45910</v>
+        <v>45934</v>
       </c>
       <c r="F24" s="16">
         <v>14</v>
@@ -13862,7 +13735,7 @@
       <c r="D25" s="92"/>
       <c r="E25" s="46">
         <f ca="1">TODAY()+35</f>
-        <v>45926</v>
+        <v>45950</v>
       </c>
       <c r="F25" s="16">
         <v>6</v>
@@ -14102,7 +13975,7 @@
       <c r="D26" s="48"/>
       <c r="E26" s="46">
         <f ca="1">TODAY()+48</f>
-        <v>45939</v>
+        <v>45963</v>
       </c>
       <c r="F26" s="16">
         <v>3</v>
@@ -14342,7 +14215,7 @@
       <c r="D27" s="92"/>
       <c r="E27" s="46">
         <f ca="1">TODAY()+40</f>
-        <v>45931</v>
+        <v>45955</v>
       </c>
       <c r="F27" s="16">
         <v>19</v>
@@ -14817,7 +14690,7 @@
       <c r="D29" s="92"/>
       <c r="E29" s="46">
         <f ca="1">TODAY()+37</f>
-        <v>45928</v>
+        <v>45952</v>
       </c>
       <c r="F29" s="16">
         <v>15</v>
@@ -15057,7 +14930,7 @@
       <c r="D30" s="48"/>
       <c r="E30" s="46">
         <f ca="1">TODAY()+29</f>
-        <v>45920</v>
+        <v>45944</v>
       </c>
       <c r="F30" s="16">
         <v>5</v>
@@ -15297,7 +15170,7 @@
       <c r="D31" s="92"/>
       <c r="E31" s="46">
         <f ca="1">TODAY()+80</f>
-        <v>45971</v>
+        <v>45995</v>
       </c>
       <c r="F31" s="16">
         <v>5</v>
@@ -17169,47 +17042,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:BK34">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="13" priority="19">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BK12 H22:BK38">
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E9+1,H$7&lt;=$E9+$F9-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK8">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>H$7&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35:BK35">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:BK36">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:BK37">
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:BK38">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:BK15">
-    <cfRule type="expression" dxfId="10" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="83" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E19+1,H$7&lt;=$E19+$F19-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:BK21">
-    <cfRule type="expression" dxfId="9" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="87" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E13+1,H$7&lt;=$E13+$F13-2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17588,7 +17461,7 @@
       </c>
       <c r="C5" s="51">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
-        <v>45888</v>
+        <v>45912</v>
       </c>
       <c r="E5" s="67"/>
       <c r="H5" s="40"/>
@@ -17597,18 +17470,18 @@
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
       <c r="M5" s="42"/>
-      <c r="O5" s="106" t="s">
+      <c r="O5" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="107">
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="119">
         <v>13</v>
       </c>
-      <c r="V5" s="107"/>
+      <c r="V5" s="119"/>
     </row>
     <row r="6" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
@@ -17634,7 +17507,7 @@
       <c r="N6" s="27"/>
       <c r="O6" s="27" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v/>
+        <v>October</v>
       </c>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
@@ -17674,7 +17547,7 @@
       <c r="AP6" s="27"/>
       <c r="AQ6" s="27" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v>October</v>
+        <v/>
       </c>
       <c r="AR6" s="27"/>
       <c r="AS6" s="27"/>
@@ -17684,7 +17557,7 @@
       <c r="AW6" s="27"/>
       <c r="AX6" s="27" t="str">
         <f ca="1">IF(OR(TEXT(AX7,"mmmm")=AQ6,TEXT(AX7,"mmmm")=AJ6,TEXT(AX7,"mmmm")=AC6,TEXT(AX7,"mmmm")=V6),"",TEXT(AX7,"mmmm"))</f>
-        <v/>
+        <v>November</v>
       </c>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="27"/>
@@ -17708,227 +17581,227 @@
       <c r="B7" s="23"/>
       <c r="H7" s="58">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>45901</v>
+        <v>45925</v>
       </c>
       <c r="I7" s="60">
         <f ca="1">H7+1</f>
-        <v>45902</v>
+        <v>45926</v>
       </c>
       <c r="J7" s="60">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>45903</v>
+        <v>45927</v>
       </c>
       <c r="K7" s="60">
         <f ca="1">J7+1</f>
-        <v>45904</v>
+        <v>45928</v>
       </c>
       <c r="L7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45905</v>
+        <v>45929</v>
       </c>
       <c r="M7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="N7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45907</v>
+        <v>45931</v>
       </c>
       <c r="O7" s="60">
         <f ca="1">N7+1</f>
-        <v>45908</v>
+        <v>45932</v>
       </c>
       <c r="P7" s="60">
         <f ca="1">O7+1</f>
-        <v>45909</v>
+        <v>45933</v>
       </c>
       <c r="Q7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45910</v>
+        <v>45934</v>
       </c>
       <c r="R7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45911</v>
+        <v>45935</v>
       </c>
       <c r="S7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45912</v>
+        <v>45936</v>
       </c>
       <c r="T7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45913</v>
+        <v>45937</v>
       </c>
       <c r="U7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45914</v>
+        <v>45938</v>
       </c>
       <c r="V7" s="60">
         <f ca="1">U7+1</f>
-        <v>45915</v>
+        <v>45939</v>
       </c>
       <c r="W7" s="60">
         <f ca="1">V7+1</f>
-        <v>45916</v>
+        <v>45940</v>
       </c>
       <c r="X7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45917</v>
+        <v>45941</v>
       </c>
       <c r="Y7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45918</v>
+        <v>45942</v>
       </c>
       <c r="Z7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45919</v>
+        <v>45943</v>
       </c>
       <c r="AA7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45920</v>
+        <v>45944</v>
       </c>
       <c r="AB7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45921</v>
+        <v>45945</v>
       </c>
       <c r="AC7" s="60">
         <f ca="1">AB7+1</f>
-        <v>45922</v>
+        <v>45946</v>
       </c>
       <c r="AD7" s="60">
         <f ca="1">AC7+1</f>
-        <v>45923</v>
+        <v>45947</v>
       </c>
       <c r="AE7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45924</v>
+        <v>45948</v>
       </c>
       <c r="AF7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45925</v>
+        <v>45949</v>
       </c>
       <c r="AG7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45926</v>
+        <v>45950</v>
       </c>
       <c r="AH7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45927</v>
+        <v>45951</v>
       </c>
       <c r="AI7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45928</v>
+        <v>45952</v>
       </c>
       <c r="AJ7" s="60">
         <f ca="1">AI7+1</f>
-        <v>45929</v>
+        <v>45953</v>
       </c>
       <c r="AK7" s="60">
         <f ca="1">AJ7+1</f>
-        <v>45930</v>
+        <v>45954</v>
       </c>
       <c r="AL7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45931</v>
+        <v>45955</v>
       </c>
       <c r="AM7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45932</v>
+        <v>45956</v>
       </c>
       <c r="AN7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45933</v>
+        <v>45957</v>
       </c>
       <c r="AO7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45934</v>
+        <v>45958</v>
       </c>
       <c r="AP7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45935</v>
+        <v>45959</v>
       </c>
       <c r="AQ7" s="60">
         <f ca="1">AP7+1</f>
-        <v>45936</v>
+        <v>45960</v>
       </c>
       <c r="AR7" s="60">
         <f ca="1">AQ7+1</f>
-        <v>45937</v>
+        <v>45961</v>
       </c>
       <c r="AS7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45938</v>
+        <v>45962</v>
       </c>
       <c r="AT7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45939</v>
+        <v>45963</v>
       </c>
       <c r="AU7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45940</v>
+        <v>45964</v>
       </c>
       <c r="AV7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45941</v>
+        <v>45965</v>
       </c>
       <c r="AW7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>45942</v>
+        <v>45966</v>
       </c>
       <c r="AX7" s="60">
         <f ca="1">AW7+1</f>
-        <v>45943</v>
+        <v>45967</v>
       </c>
       <c r="AY7" s="60">
         <f ca="1">AX7+1</f>
-        <v>45944</v>
+        <v>45968</v>
       </c>
       <c r="AZ7" s="60">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>45945</v>
+        <v>45969</v>
       </c>
       <c r="BA7" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>45946</v>
+        <v>45970</v>
       </c>
       <c r="BB7" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>45947</v>
+        <v>45971</v>
       </c>
       <c r="BC7" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>45948</v>
+        <v>45972</v>
       </c>
       <c r="BD7" s="60">
         <f t="shared" ca="1" si="1"/>
-        <v>45949</v>
+        <v>45973</v>
       </c>
       <c r="BE7" s="60">
         <f ca="1">BD7+1</f>
-        <v>45950</v>
+        <v>45974</v>
       </c>
       <c r="BF7" s="60">
         <f ca="1">BE7+1</f>
-        <v>45951</v>
+        <v>45975</v>
       </c>
       <c r="BG7" s="60">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>45952</v>
+        <v>45976</v>
       </c>
       <c r="BH7" s="60">
         <f t="shared" ca="1" si="2"/>
-        <v>45953</v>
+        <v>45977</v>
       </c>
       <c r="BI7" s="60">
         <f t="shared" ca="1" si="2"/>
-        <v>45954</v>
+        <v>45978</v>
       </c>
       <c r="BJ7" s="60">
         <f t="shared" ca="1" si="2"/>
-        <v>45955</v>
+        <v>45979</v>
       </c>
       <c r="BK7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>45956</v>
+        <v>45980</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="31" customHeight="1" x14ac:dyDescent="0.35">
@@ -17951,227 +17824,227 @@
       <c r="G8" s="63"/>
       <c r="H8" s="62" t="str">
         <f ca="1">LEFT(TEXT(H7,"ddd"),1)</f>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="I8" s="61" t="str">
         <f ca="1">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="J8" s="61" t="str">
         <f ca="1">LEFT(TEXT(J7,"ddd"),1)</f>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="K8" s="61" t="str">
         <f t="shared" ref="K8:AM8" ca="1" si="3">LEFT(TEXT(K7,"ddd"),1)</f>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="L8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="M8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="N8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="O8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="P8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="Q8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="R8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="S8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="T8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="U8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="V8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="W8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="X8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="Y8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="Z8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AA8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AB8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AC8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AD8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AE8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AF8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AG8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AH8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AI8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AJ8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AK8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AL8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AM8" s="61" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AN8" s="61" t="str">
         <f t="shared" ref="AN8:BK8" ca="1" si="4">LEFT(TEXT(AN7,"ddd"),1)</f>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AO8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AP8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AQ8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AR8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AS8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AT8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AU8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AV8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AW8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AX8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="AY8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="AZ8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BA8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BB8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BC8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BD8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BE8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>T</v>
       </c>
       <c r="BF8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>F</v>
       </c>
       <c r="BG8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BH8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BI8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BJ8" s="61" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BK8" s="59" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>W</v>
       </c>
     </row>
     <row r="9" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -18483,7 +18356,7 @@
       </c>
       <c r="E11" s="46">
         <f ca="1">TODAY()</f>
-        <v>45891</v>
+        <v>45915</v>
       </c>
       <c r="F11" s="16">
         <v>3</v>
@@ -18723,7 +18596,7 @@
       <c r="D12" s="47"/>
       <c r="E12" s="46">
         <f ca="1">TODAY()+5</f>
-        <v>45896</v>
+        <v>45920</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
@@ -18965,7 +18838,7 @@
       </c>
       <c r="E13" s="46">
         <f ca="1">TODAY()-3</f>
-        <v>45888</v>
+        <v>45912</v>
       </c>
       <c r="F13" s="16">
         <v>10</v>
@@ -19205,7 +19078,7 @@
       <c r="D14" s="47"/>
       <c r="E14" s="46">
         <f ca="1">TODAY()+20</f>
-        <v>45911</v>
+        <v>45935</v>
       </c>
       <c r="F14" s="16">
         <v>1</v>
@@ -19447,7 +19320,7 @@
       </c>
       <c r="E15" s="46">
         <f ca="1">TODAY()+6</f>
-        <v>45897</v>
+        <v>45921</v>
       </c>
       <c r="F15" s="16">
         <v>6</v>
@@ -19924,7 +19797,7 @@
       </c>
       <c r="E17" s="46">
         <f ca="1">TODAY()+6</f>
-        <v>45897</v>
+        <v>45921</v>
       </c>
       <c r="F17" s="16">
         <v>13</v>
@@ -20166,7 +20039,7 @@
       </c>
       <c r="E18" s="46">
         <f ca="1">TODAY()+7</f>
-        <v>45898</v>
+        <v>45922</v>
       </c>
       <c r="F18" s="16">
         <v>9</v>
@@ -20408,7 +20281,7 @@
       </c>
       <c r="E19" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F19" s="16">
         <v>11</v>
@@ -20648,7 +20521,7 @@
       <c r="D20" s="47"/>
       <c r="E20" s="46">
         <f ca="1">TODAY()+24</f>
-        <v>45915</v>
+        <v>45939</v>
       </c>
       <c r="F20" s="16">
         <v>1</v>
@@ -20888,7 +20761,7 @@
       <c r="D21" s="47"/>
       <c r="E21" s="46">
         <f ca="1">TODAY()+25</f>
-        <v>45916</v>
+        <v>45940</v>
       </c>
       <c r="F21" s="16">
         <v>24</v>
@@ -21363,7 +21236,7 @@
       <c r="D23" s="47"/>
       <c r="E23" s="46">
         <f ca="1">TODAY()+15</f>
-        <v>45906</v>
+        <v>45930</v>
       </c>
       <c r="F23" s="16">
         <v>4</v>
@@ -21603,7 +21476,7 @@
       <c r="D24" s="47"/>
       <c r="E24" s="46">
         <f ca="1">TODAY()+19</f>
-        <v>45910</v>
+        <v>45934</v>
       </c>
       <c r="F24" s="16">
         <v>14</v>
@@ -21843,7 +21716,7 @@
       <c r="D25" s="47"/>
       <c r="E25" s="46">
         <f ca="1">TODAY()+35</f>
-        <v>45926</v>
+        <v>45950</v>
       </c>
       <c r="F25" s="16">
         <v>6</v>
@@ -22083,7 +21956,7 @@
       <c r="D26" s="47"/>
       <c r="E26" s="46">
         <f ca="1">TODAY()+48</f>
-        <v>45939</v>
+        <v>45963</v>
       </c>
       <c r="F26" s="16">
         <v>3</v>
@@ -22323,7 +22196,7 @@
       <c r="D27" s="47"/>
       <c r="E27" s="46">
         <f ca="1">TODAY()+40</f>
-        <v>45931</v>
+        <v>45955</v>
       </c>
       <c r="F27" s="16">
         <v>19</v>
@@ -22798,7 +22671,7 @@
       <c r="D29" s="47"/>
       <c r="E29" s="46">
         <f ca="1">TODAY()+37</f>
-        <v>45928</v>
+        <v>45952</v>
       </c>
       <c r="F29" s="16">
         <v>15</v>
@@ -23038,7 +22911,7 @@
       <c r="D30" s="47"/>
       <c r="E30" s="46">
         <f ca="1">TODAY()+29</f>
-        <v>45920</v>
+        <v>45944</v>
       </c>
       <c r="F30" s="16">
         <v>5</v>
@@ -23278,7 +23151,7 @@
       <c r="D31" s="47"/>
       <c r="E31" s="46">
         <f ca="1">TODAY()+80</f>
-        <v>45971</v>
+        <v>45995</v>
       </c>
       <c r="F31" s="16">
         <v>5</v>
@@ -24307,17 +24180,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:BK34">
-    <cfRule type="expression" dxfId="20" priority="78">
+    <cfRule type="expression" dxfId="3" priority="78">
       <formula>H$7&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BK34">
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
       <formula>AND(H$7&gt;=$E9+1,H$7&lt;=$E9+$F9-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK8">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>H$7&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24434,6 +24307,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24733,36 +24635,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{115E488A-90BD-4FEC-9F20-FFAF098D38E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8EE784-10F3-46EF-B6DC-D206373B3A17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D999942B-3CC5-4007-B7B6-6870B5EC1C9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24783,26 +24676,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8EE784-10F3-46EF-B6DC-D206373B3A17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{115E488A-90BD-4FEC-9F20-FFAF098D38E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>